<commit_message>
Utcamp form finished, batch is appiable added.
</commit_message>
<xml_diff>
--- a/docs/tcamp/2022教師營_程式希求1007-給允中.xlsx
+++ b/docs/tcamp/2022教師營_程式希求1007-給允中.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bwcamp\docs\tcamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lzong/wwwroot/bwcamp/docs/tcamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188127E8-59A3-41A3-B928-D9CECC6C0C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80534A7A-EFFF-0A49-BB6C-1AD5F4810B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14780" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -403,7 +403,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -628,6 +628,15 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,13 +656,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -937,39 +940,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36.3984375" customWidth="1"/>
+    <col min="2" max="2" width="21.796875" customWidth="1"/>
+    <col min="3" max="3" width="17.19921875" customWidth="1"/>
+    <col min="4" max="4" width="15.796875" customWidth="1"/>
+    <col min="5" max="5" width="12.59765625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.3984375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:8" ht="22" customHeight="1">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="38" customHeight="1">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-    </row>
-    <row r="3" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="22" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -977,62 +980,62 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:8" ht="22" customHeight="1">
+      <c r="A4" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:8" ht="33.5" customHeight="1">
+      <c r="A5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:8" ht="99" customHeight="1">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+    <row r="7" spans="1:8" ht="21.5" customHeight="1">
+      <c r="A7" s="23" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:8" ht="21" customHeight="1">
+      <c r="A8" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:8" ht="75" customHeight="1">
+      <c r="A9" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:8" ht="24.5" customHeight="1">
+      <c r="A10" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1048,28 +1051,28 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="138.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22" t="s">
+    <row r="11" spans="1:8" ht="139" customHeight="1">
+      <c r="A11" s="26"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="24" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="21"/>
+    <row r="12" spans="1:8" ht="35.5" customHeight="1">
+      <c r="A12" s="26"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="8" t="s">
         <v>17</v>
       </c>
@@ -1080,10 +1083,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
+    <row r="13" spans="1:8" ht="136.5" customHeight="1">
+      <c r="A13" s="26"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="17" t="s">
         <v>21</v>
       </c>
@@ -1094,8 +1097,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+    <row r="14" spans="1:8" ht="28" customHeight="1">
+      <c r="A14" s="26"/>
       <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
@@ -1106,12 +1109,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="23.5" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="24" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>25</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="62" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>34</v>
       </c>
@@ -1136,25 +1139,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="24" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="24" customHeight="1">
       <c r="A19" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
+    <row r="20" spans="1:5" ht="47.5" customHeight="1">
+      <c r="A20" s="30" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="24" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>33</v>
       </c>
@@ -1162,13 +1165,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:5" ht="24" customHeight="1">
+      <c r="A22" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="14"/>
     </row>
-    <row r="23" spans="1:5" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="38" customHeight="1">
       <c r="A23" s="5" t="s">
         <v>37</v>
       </c>
@@ -1176,7 +1179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="115" customHeight="1">
       <c r="A24" s="12" t="s">
         <v>38</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="158.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="158.5" customHeight="1">
       <c r="A25" s="12" t="s">
         <v>40</v>
       </c>
@@ -1192,17 +1195,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="27.5" customHeight="1">
       <c r="A26" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="27.5" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="26.5" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>42</v>
       </c>

</xml_diff>